<commit_message>
did some data processing in excel
</commit_message>
<xml_diff>
--- a/OvenTests/40DutyCycleAndCooldown.xlsx
+++ b/OvenTests/40DutyCycleAndCooldown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlols\OneDrive\Desktop\Schoolwork\9. Small Sat Research Lab\SSRLReflowOven\OvenTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78AACC5-1680-461F-A56C-398102460820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13130F0C-A10F-4977-A556-4D1704242909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B63B50FC-0F95-44DF-9245-6F363CF8556D}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Time</t>
   </si>
   <si>
     <t>Temperature (C)</t>
+  </si>
+  <si>
+    <t>Max slope range</t>
   </si>
 </sst>
 </file>
@@ -28276,6 +28279,1085 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1660275798858476"/>
+                  <c:y val="-0.16947822350608541"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$21:$D$143</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="123"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>68.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>75.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>77.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>81.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>84.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>91.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>93.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>100.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>101.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>102.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>105.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>106.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>108.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>110.51</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>111.01</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>111.51</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>112.01</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>112.51</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>113.01</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>113.51</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>114.01</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>114.51</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>115.01</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>115.51</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>116.01</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>116.51</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>117.01</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>117.51</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>118.01</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118.51</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119.01</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>119.51</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>120.01</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>120.51</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>121.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$21:$E$143</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="123"/>
+                <c:pt idx="0">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>48.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48.75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>48.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>49.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>49.75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>50.75</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>51.25</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>51.75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>52.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>52.75</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>53.25</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>54.25</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>54.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>54.75</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>55.75</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>56.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>56.75</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>57.25</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>57.75</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>58.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>58.75</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>59.25</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>59.75</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>60.25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60.75</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61.25</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>61.5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>61.75</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>62.25</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>62.75</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>63.75</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>64.25</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>64.75</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>65.25</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>65.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>66.75</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>67.75</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>68.25</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>68.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>68.75</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>69.25</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>70.25</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>70.75</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>71.25</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>71.75</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>72.25</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>73.25</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>73.75</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>74.25</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>74.75</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>75.25</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>75.5</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>75.75</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>76.25</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>76.75</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>77.25</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>77.5</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>77.75</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>78.75</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>79.25</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>79.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6687-43EB-8068-16F24AB0E20E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1155791711"/>
+        <c:axId val="1155787551"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1155791711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155787551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1155787551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155791711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -28317,6 +29399,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -29388,6 +30510,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -29457,6 +31095,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8216BAC5-3007-4968-AEEC-164490A51417}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -29765,7 +31439,7 @@
   <dimension ref="A1:K3002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -30043,6 +31717,9 @@
       <c r="B20">
         <v>31.5</v>
       </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
       <c r="J20">
         <v>9.5</v>
       </c>
@@ -30057,6 +31734,12 @@
       <c r="B21">
         <v>31.5</v>
       </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <v>44</v>
+      </c>
       <c r="J21">
         <v>10</v>
       </c>
@@ -30071,6 +31754,12 @@
       <c r="B22">
         <v>31.5</v>
       </c>
+      <c r="D22">
+        <v>60.5</v>
+      </c>
+      <c r="E22">
+        <v>44.25</v>
+      </c>
       <c r="J22">
         <v>10.5</v>
       </c>
@@ -30085,6 +31774,12 @@
       <c r="B23">
         <v>31.5</v>
       </c>
+      <c r="D23">
+        <v>61</v>
+      </c>
+      <c r="E23">
+        <v>44.5</v>
+      </c>
       <c r="J23">
         <v>11</v>
       </c>
@@ -30099,6 +31794,12 @@
       <c r="B24">
         <v>31.5</v>
       </c>
+      <c r="D24">
+        <v>61.5</v>
+      </c>
+      <c r="E24">
+        <v>44.75</v>
+      </c>
       <c r="J24">
         <v>11.5</v>
       </c>
@@ -30113,6 +31814,12 @@
       <c r="B25">
         <v>31.75</v>
       </c>
+      <c r="D25">
+        <v>62</v>
+      </c>
+      <c r="E25">
+        <v>45</v>
+      </c>
       <c r="J25">
         <v>12</v>
       </c>
@@ -30127,6 +31834,12 @@
       <c r="B26">
         <v>31.5</v>
       </c>
+      <c r="D26">
+        <v>62.5</v>
+      </c>
+      <c r="E26">
+        <v>45.25</v>
+      </c>
       <c r="J26">
         <v>12.5</v>
       </c>
@@ -30141,6 +31854,12 @@
       <c r="B27">
         <v>31.5</v>
       </c>
+      <c r="D27">
+        <v>63</v>
+      </c>
+      <c r="E27">
+        <v>45.5</v>
+      </c>
       <c r="J27">
         <v>13</v>
       </c>
@@ -30155,6 +31874,12 @@
       <c r="B28">
         <v>31.75</v>
       </c>
+      <c r="D28">
+        <v>63.5</v>
+      </c>
+      <c r="E28">
+        <v>45.75</v>
+      </c>
       <c r="J28">
         <v>13.5</v>
       </c>
@@ -30169,6 +31894,12 @@
       <c r="B29">
         <v>31.5</v>
       </c>
+      <c r="D29">
+        <v>64</v>
+      </c>
+      <c r="E29">
+        <v>46</v>
+      </c>
       <c r="J29">
         <v>14</v>
       </c>
@@ -30183,6 +31914,12 @@
       <c r="B30">
         <v>31.5</v>
       </c>
+      <c r="D30">
+        <v>64.5</v>
+      </c>
+      <c r="E30">
+        <v>46.25</v>
+      </c>
       <c r="J30">
         <v>14.5</v>
       </c>
@@ -30197,6 +31934,12 @@
       <c r="B31">
         <v>31.5</v>
       </c>
+      <c r="D31">
+        <v>65</v>
+      </c>
+      <c r="E31">
+        <v>46.5</v>
+      </c>
       <c r="J31">
         <v>15</v>
       </c>
@@ -30211,6 +31954,12 @@
       <c r="B32">
         <v>31.75</v>
       </c>
+      <c r="D32">
+        <v>65.5</v>
+      </c>
+      <c r="E32">
+        <v>46.75</v>
+      </c>
       <c r="J32">
         <v>15.5</v>
       </c>
@@ -30225,6 +31974,12 @@
       <c r="B33">
         <v>31.75</v>
       </c>
+      <c r="D33">
+        <v>66</v>
+      </c>
+      <c r="E33">
+        <v>47</v>
+      </c>
       <c r="J33">
         <v>16</v>
       </c>
@@ -30239,6 +31994,12 @@
       <c r="B34">
         <v>31.75</v>
       </c>
+      <c r="D34">
+        <v>66.5</v>
+      </c>
+      <c r="E34">
+        <v>47.25</v>
+      </c>
       <c r="J34">
         <v>16.5</v>
       </c>
@@ -30253,6 +32014,12 @@
       <c r="B35">
         <v>31.75</v>
       </c>
+      <c r="D35">
+        <v>67</v>
+      </c>
+      <c r="E35">
+        <v>47.5</v>
+      </c>
       <c r="J35">
         <v>17</v>
       </c>
@@ -30267,6 +32034,12 @@
       <c r="B36">
         <v>32</v>
       </c>
+      <c r="D36">
+        <v>67.5</v>
+      </c>
+      <c r="E36">
+        <v>47.75</v>
+      </c>
       <c r="J36">
         <v>17.5</v>
       </c>
@@ -30281,6 +32054,12 @@
       <c r="B37">
         <v>31.75</v>
       </c>
+      <c r="D37">
+        <v>68</v>
+      </c>
+      <c r="E37">
+        <v>48.25</v>
+      </c>
       <c r="J37">
         <v>18</v>
       </c>
@@ -30295,6 +32074,12 @@
       <c r="B38">
         <v>31.75</v>
       </c>
+      <c r="D38">
+        <v>68.5</v>
+      </c>
+      <c r="E38">
+        <v>48.25</v>
+      </c>
       <c r="J38">
         <v>18.5</v>
       </c>
@@ -30309,6 +32094,12 @@
       <c r="B39">
         <v>32</v>
       </c>
+      <c r="D39">
+        <v>69</v>
+      </c>
+      <c r="E39">
+        <v>48.75</v>
+      </c>
       <c r="J39">
         <v>19</v>
       </c>
@@ -30323,6 +32114,12 @@
       <c r="B40">
         <v>32</v>
       </c>
+      <c r="D40">
+        <v>69.5</v>
+      </c>
+      <c r="E40">
+        <v>48.75</v>
+      </c>
       <c r="J40">
         <v>19.5</v>
       </c>
@@ -30337,6 +32134,12 @@
       <c r="B41">
         <v>32</v>
       </c>
+      <c r="D41">
+        <v>70</v>
+      </c>
+      <c r="E41">
+        <v>49.25</v>
+      </c>
       <c r="J41">
         <v>20</v>
       </c>
@@ -30351,6 +32154,12 @@
       <c r="B42">
         <v>32</v>
       </c>
+      <c r="D42">
+        <v>70.5</v>
+      </c>
+      <c r="E42">
+        <v>49.25</v>
+      </c>
       <c r="J42">
         <v>20.5</v>
       </c>
@@ -30365,6 +32174,12 @@
       <c r="B43">
         <v>32</v>
       </c>
+      <c r="D43">
+        <v>71</v>
+      </c>
+      <c r="E43">
+        <v>49.75</v>
+      </c>
       <c r="J43">
         <v>21</v>
       </c>
@@ -30379,6 +32194,12 @@
       <c r="B44">
         <v>32.25</v>
       </c>
+      <c r="D44">
+        <v>71.5</v>
+      </c>
+      <c r="E44">
+        <v>50</v>
+      </c>
       <c r="J44">
         <v>21.5</v>
       </c>
@@ -30393,6 +32214,12 @@
       <c r="B45">
         <v>32.25</v>
       </c>
+      <c r="D45">
+        <v>72</v>
+      </c>
+      <c r="E45">
+        <v>50.25</v>
+      </c>
       <c r="J45">
         <v>22</v>
       </c>
@@ -30407,6 +32234,12 @@
       <c r="B46">
         <v>32.25</v>
       </c>
+      <c r="D46">
+        <v>72.5</v>
+      </c>
+      <c r="E46">
+        <v>50.5</v>
+      </c>
       <c r="J46">
         <v>22.5</v>
       </c>
@@ -30421,6 +32254,12 @@
       <c r="B47">
         <v>32.5</v>
       </c>
+      <c r="D47">
+        <v>73</v>
+      </c>
+      <c r="E47">
+        <v>50.75</v>
+      </c>
       <c r="J47">
         <v>23</v>
       </c>
@@ -30435,6 +32274,12 @@
       <c r="B48">
         <v>32.25</v>
       </c>
+      <c r="D48">
+        <v>73.5</v>
+      </c>
+      <c r="E48">
+        <v>51</v>
+      </c>
       <c r="J48">
         <v>23.5</v>
       </c>
@@ -30449,6 +32294,12 @@
       <c r="B49">
         <v>32.5</v>
       </c>
+      <c r="D49">
+        <v>74</v>
+      </c>
+      <c r="E49">
+        <v>51.25</v>
+      </c>
       <c r="J49">
         <v>24</v>
       </c>
@@ -30463,6 +32314,12 @@
       <c r="B50">
         <v>32.75</v>
       </c>
+      <c r="D50">
+        <v>74.5</v>
+      </c>
+      <c r="E50">
+        <v>51.5</v>
+      </c>
       <c r="J50">
         <v>24.5</v>
       </c>
@@ -30477,6 +32334,12 @@
       <c r="B51">
         <v>32.75</v>
       </c>
+      <c r="D51">
+        <v>75</v>
+      </c>
+      <c r="E51">
+        <v>51.75</v>
+      </c>
       <c r="J51">
         <v>25</v>
       </c>
@@ -30491,6 +32354,12 @@
       <c r="B52">
         <v>32.75</v>
       </c>
+      <c r="D52">
+        <v>75.5</v>
+      </c>
+      <c r="E52">
+        <v>52.25</v>
+      </c>
       <c r="J52">
         <v>25.5</v>
       </c>
@@ -30505,6 +32374,12 @@
       <c r="B53">
         <v>32.75</v>
       </c>
+      <c r="D53">
+        <v>76</v>
+      </c>
+      <c r="E53">
+        <v>52.5</v>
+      </c>
       <c r="J53">
         <v>26</v>
       </c>
@@ -30519,6 +32394,12 @@
       <c r="B54">
         <v>32.75</v>
       </c>
+      <c r="D54">
+        <v>76.5</v>
+      </c>
+      <c r="E54">
+        <v>52.75</v>
+      </c>
       <c r="J54">
         <v>26.5</v>
       </c>
@@ -30533,6 +32414,12 @@
       <c r="B55">
         <v>33</v>
       </c>
+      <c r="D55">
+        <v>77</v>
+      </c>
+      <c r="E55">
+        <v>53</v>
+      </c>
       <c r="J55">
         <v>27</v>
       </c>
@@ -30547,6 +32434,12 @@
       <c r="B56">
         <v>33</v>
       </c>
+      <c r="D56">
+        <v>77.5</v>
+      </c>
+      <c r="E56">
+        <v>53.25</v>
+      </c>
       <c r="J56">
         <v>27.5</v>
       </c>
@@ -30561,6 +32454,12 @@
       <c r="B57">
         <v>33.25</v>
       </c>
+      <c r="D57">
+        <v>78</v>
+      </c>
+      <c r="E57">
+        <v>53.5</v>
+      </c>
       <c r="J57">
         <v>28</v>
       </c>
@@ -30575,6 +32474,12 @@
       <c r="B58">
         <v>33.25</v>
       </c>
+      <c r="D58">
+        <v>78.5</v>
+      </c>
+      <c r="E58">
+        <v>54</v>
+      </c>
       <c r="J58">
         <v>28.5</v>
       </c>
@@ -30589,6 +32494,12 @@
       <c r="B59">
         <v>33.5</v>
       </c>
+      <c r="D59">
+        <v>79</v>
+      </c>
+      <c r="E59">
+        <v>54.25</v>
+      </c>
       <c r="J59">
         <v>29</v>
       </c>
@@ -30603,6 +32514,12 @@
       <c r="B60">
         <v>33.5</v>
       </c>
+      <c r="D60">
+        <v>79.5</v>
+      </c>
+      <c r="E60">
+        <v>54.5</v>
+      </c>
       <c r="J60">
         <v>29.5</v>
       </c>
@@ -30617,6 +32534,12 @@
       <c r="B61">
         <v>33.75</v>
       </c>
+      <c r="D61">
+        <v>80</v>
+      </c>
+      <c r="E61">
+        <v>54.75</v>
+      </c>
       <c r="J61">
         <v>30</v>
       </c>
@@ -30631,6 +32554,12 @@
       <c r="B62">
         <v>33.75</v>
       </c>
+      <c r="D62">
+        <v>80.5</v>
+      </c>
+      <c r="E62">
+        <v>55</v>
+      </c>
       <c r="J62">
         <v>30.5</v>
       </c>
@@ -30645,6 +32574,12 @@
       <c r="B63">
         <v>34</v>
       </c>
+      <c r="D63">
+        <v>81</v>
+      </c>
+      <c r="E63">
+        <v>55.5</v>
+      </c>
       <c r="J63">
         <v>31</v>
       </c>
@@ -30659,6 +32594,12 @@
       <c r="B64">
         <v>34</v>
       </c>
+      <c r="D64">
+        <v>81.5</v>
+      </c>
+      <c r="E64">
+        <v>55.75</v>
+      </c>
       <c r="J64">
         <v>31.5</v>
       </c>
@@ -30673,6 +32614,12 @@
       <c r="B65">
         <v>34</v>
       </c>
+      <c r="D65">
+        <v>82</v>
+      </c>
+      <c r="E65">
+        <v>56</v>
+      </c>
       <c r="J65">
         <v>32</v>
       </c>
@@ -30687,6 +32634,12 @@
       <c r="B66">
         <v>34.25</v>
       </c>
+      <c r="D66">
+        <v>82.5</v>
+      </c>
+      <c r="E66">
+        <v>56.5</v>
+      </c>
       <c r="J66">
         <v>32.5</v>
       </c>
@@ -30701,6 +32654,12 @@
       <c r="B67">
         <v>34.25</v>
       </c>
+      <c r="D67">
+        <v>83</v>
+      </c>
+      <c r="E67">
+        <v>56.75</v>
+      </c>
       <c r="J67">
         <v>33</v>
       </c>
@@ -30715,6 +32674,12 @@
       <c r="B68">
         <v>34.25</v>
       </c>
+      <c r="D68">
+        <v>83.5</v>
+      </c>
+      <c r="E68">
+        <v>57</v>
+      </c>
       <c r="J68">
         <v>33.5</v>
       </c>
@@ -30729,6 +32694,12 @@
       <c r="B69">
         <v>34.5</v>
       </c>
+      <c r="D69">
+        <v>84</v>
+      </c>
+      <c r="E69">
+        <v>57.25</v>
+      </c>
       <c r="J69">
         <v>34</v>
       </c>
@@ -30743,6 +32714,12 @@
       <c r="B70">
         <v>34.5</v>
       </c>
+      <c r="D70">
+        <v>84.5</v>
+      </c>
+      <c r="E70">
+        <v>57.5</v>
+      </c>
       <c r="J70">
         <v>34.5</v>
       </c>
@@ -30757,6 +32734,12 @@
       <c r="B71">
         <v>34.5</v>
       </c>
+      <c r="D71">
+        <v>85</v>
+      </c>
+      <c r="E71">
+        <v>57.75</v>
+      </c>
       <c r="J71">
         <v>35</v>
       </c>
@@ -30771,6 +32754,12 @@
       <c r="B72">
         <v>34.75</v>
       </c>
+      <c r="D72">
+        <v>85.5</v>
+      </c>
+      <c r="E72">
+        <v>58</v>
+      </c>
       <c r="J72">
         <v>35.5</v>
       </c>
@@ -30785,6 +32774,12 @@
       <c r="B73">
         <v>35</v>
       </c>
+      <c r="D73">
+        <v>86</v>
+      </c>
+      <c r="E73">
+        <v>58.5</v>
+      </c>
       <c r="J73">
         <v>36</v>
       </c>
@@ -30799,6 +32794,12 @@
       <c r="B74">
         <v>35</v>
       </c>
+      <c r="D74">
+        <v>86.5</v>
+      </c>
+      <c r="E74">
+        <v>58.75</v>
+      </c>
       <c r="J74">
         <v>36.5</v>
       </c>
@@ -30813,6 +32814,12 @@
       <c r="B75">
         <v>35.25</v>
       </c>
+      <c r="D75">
+        <v>87</v>
+      </c>
+      <c r="E75">
+        <v>59</v>
+      </c>
       <c r="J75">
         <v>37</v>
       </c>
@@ -30827,6 +32834,12 @@
       <c r="B76">
         <v>35.5</v>
       </c>
+      <c r="D76">
+        <v>87.5</v>
+      </c>
+      <c r="E76">
+        <v>59.25</v>
+      </c>
       <c r="J76">
         <v>37.5</v>
       </c>
@@ -30841,6 +32854,12 @@
       <c r="B77">
         <v>35.5</v>
       </c>
+      <c r="D77">
+        <v>88</v>
+      </c>
+      <c r="E77">
+        <v>59.75</v>
+      </c>
       <c r="J77">
         <v>38</v>
       </c>
@@ -30855,6 +32874,12 @@
       <c r="B78">
         <v>35.75</v>
       </c>
+      <c r="D78">
+        <v>88.5</v>
+      </c>
+      <c r="E78">
+        <v>60</v>
+      </c>
       <c r="J78">
         <v>38.5</v>
       </c>
@@ -30869,6 +32894,12 @@
       <c r="B79">
         <v>35.75</v>
       </c>
+      <c r="D79">
+        <v>89</v>
+      </c>
+      <c r="E79">
+        <v>60.25</v>
+      </c>
       <c r="J79">
         <v>39</v>
       </c>
@@ -30883,6 +32914,12 @@
       <c r="B80">
         <v>36</v>
       </c>
+      <c r="D80">
+        <v>89.5</v>
+      </c>
+      <c r="E80">
+        <v>60.5</v>
+      </c>
       <c r="J80">
         <v>39.5</v>
       </c>
@@ -30897,6 +32934,12 @@
       <c r="B81">
         <v>36.25</v>
       </c>
+      <c r="D81">
+        <v>90</v>
+      </c>
+      <c r="E81">
+        <v>60.75</v>
+      </c>
       <c r="J81">
         <v>40</v>
       </c>
@@ -30911,6 +32954,12 @@
       <c r="B82">
         <v>36.5</v>
       </c>
+      <c r="D82">
+        <v>90.5</v>
+      </c>
+      <c r="E82">
+        <v>61.25</v>
+      </c>
       <c r="J82">
         <v>40.5</v>
       </c>
@@ -30925,6 +32974,12 @@
       <c r="B83">
         <v>36.5</v>
       </c>
+      <c r="D83">
+        <v>91</v>
+      </c>
+      <c r="E83">
+        <v>61.5</v>
+      </c>
       <c r="J83">
         <v>41</v>
       </c>
@@ -30939,6 +32994,12 @@
       <c r="B84">
         <v>36.75</v>
       </c>
+      <c r="D84">
+        <v>91.5</v>
+      </c>
+      <c r="E84">
+        <v>61.75</v>
+      </c>
       <c r="J84">
         <v>41.5</v>
       </c>
@@ -30953,6 +33014,12 @@
       <c r="B85">
         <v>36.75</v>
       </c>
+      <c r="D85">
+        <v>92</v>
+      </c>
+      <c r="E85">
+        <v>62.25</v>
+      </c>
       <c r="J85">
         <v>42</v>
       </c>
@@ -30967,6 +33034,12 @@
       <c r="B86">
         <v>37.25</v>
       </c>
+      <c r="D86">
+        <v>92.5</v>
+      </c>
+      <c r="E86">
+        <v>62.5</v>
+      </c>
       <c r="J86">
         <v>42.5</v>
       </c>
@@ -30981,6 +33054,12 @@
       <c r="B87">
         <v>37.25</v>
       </c>
+      <c r="D87">
+        <v>93</v>
+      </c>
+      <c r="E87">
+        <v>62.75</v>
+      </c>
       <c r="J87">
         <v>43</v>
       </c>
@@ -30995,6 +33074,12 @@
       <c r="B88">
         <v>37.5</v>
       </c>
+      <c r="D88">
+        <v>93.5</v>
+      </c>
+      <c r="E88">
+        <v>63</v>
+      </c>
       <c r="J88">
         <v>43.5</v>
       </c>
@@ -31009,6 +33094,12 @@
       <c r="B89">
         <v>37.75</v>
       </c>
+      <c r="D89">
+        <v>94</v>
+      </c>
+      <c r="E89">
+        <v>63.5</v>
+      </c>
       <c r="J89">
         <v>44</v>
       </c>
@@ -31023,6 +33114,12 @@
       <c r="B90">
         <v>37.75</v>
       </c>
+      <c r="D90">
+        <v>94.5</v>
+      </c>
+      <c r="E90">
+        <v>63.75</v>
+      </c>
       <c r="J90">
         <v>44.5</v>
       </c>
@@ -31037,6 +33134,12 @@
       <c r="B91">
         <v>37.75</v>
       </c>
+      <c r="D91">
+        <v>95</v>
+      </c>
+      <c r="E91">
+        <v>64</v>
+      </c>
       <c r="J91">
         <v>45</v>
       </c>
@@ -31051,6 +33154,12 @@
       <c r="B92">
         <v>38.25</v>
       </c>
+      <c r="D92">
+        <v>95.5</v>
+      </c>
+      <c r="E92">
+        <v>64.25</v>
+      </c>
       <c r="J92">
         <v>45.5</v>
       </c>
@@ -31065,6 +33174,12 @@
       <c r="B93">
         <v>38.25</v>
       </c>
+      <c r="D93">
+        <v>96</v>
+      </c>
+      <c r="E93">
+        <v>64.75</v>
+      </c>
       <c r="J93">
         <v>46</v>
       </c>
@@ -31079,6 +33194,12 @@
       <c r="B94">
         <v>38.5</v>
       </c>
+      <c r="D94">
+        <v>96.5</v>
+      </c>
+      <c r="E94">
+        <v>65</v>
+      </c>
       <c r="J94">
         <v>46.5</v>
       </c>
@@ -31093,6 +33214,12 @@
       <c r="B95">
         <v>38.75</v>
       </c>
+      <c r="D95">
+        <v>97</v>
+      </c>
+      <c r="E95">
+        <v>65.25</v>
+      </c>
       <c r="J95">
         <v>47</v>
       </c>
@@ -31107,6 +33234,12 @@
       <c r="B96">
         <v>38.75</v>
       </c>
+      <c r="D96">
+        <v>97.5</v>
+      </c>
+      <c r="E96">
+        <v>65.5</v>
+      </c>
       <c r="J96">
         <v>47.5</v>
       </c>
@@ -31121,6 +33254,12 @@
       <c r="B97">
         <v>39</v>
       </c>
+      <c r="D97">
+        <v>98</v>
+      </c>
+      <c r="E97">
+        <v>66</v>
+      </c>
       <c r="J97">
         <v>48</v>
       </c>
@@ -31135,6 +33274,12 @@
       <c r="B98">
         <v>39.25</v>
       </c>
+      <c r="D98">
+        <v>98.5</v>
+      </c>
+      <c r="E98">
+        <v>66</v>
+      </c>
       <c r="J98">
         <v>48.5</v>
       </c>
@@ -31149,6 +33294,12 @@
       <c r="B99">
         <v>39.25</v>
       </c>
+      <c r="D99">
+        <v>99</v>
+      </c>
+      <c r="E99">
+        <v>66.5</v>
+      </c>
       <c r="J99">
         <v>49</v>
       </c>
@@ -31163,6 +33314,12 @@
       <c r="B100">
         <v>39.5</v>
       </c>
+      <c r="D100">
+        <v>99.5</v>
+      </c>
+      <c r="E100">
+        <v>66.75</v>
+      </c>
       <c r="J100">
         <v>49.5</v>
       </c>
@@ -31177,6 +33334,12 @@
       <c r="B101">
         <v>39.75</v>
       </c>
+      <c r="D101">
+        <v>100</v>
+      </c>
+      <c r="E101">
+        <v>67</v>
+      </c>
       <c r="J101">
         <v>50</v>
       </c>
@@ -31191,6 +33354,12 @@
       <c r="B102">
         <v>40</v>
       </c>
+      <c r="D102">
+        <v>100.5</v>
+      </c>
+      <c r="E102">
+        <v>67.5</v>
+      </c>
       <c r="J102">
         <v>50.5</v>
       </c>
@@ -31205,6 +33374,12 @@
       <c r="B103">
         <v>40</v>
       </c>
+      <c r="D103">
+        <v>101</v>
+      </c>
+      <c r="E103">
+        <v>67.75</v>
+      </c>
       <c r="J103">
         <v>51</v>
       </c>
@@ -31219,6 +33394,12 @@
       <c r="B104">
         <v>40.25</v>
       </c>
+      <c r="D104">
+        <v>101.5</v>
+      </c>
+      <c r="E104">
+        <v>68</v>
+      </c>
       <c r="J104">
         <v>51.5</v>
       </c>
@@ -31233,6 +33414,12 @@
       <c r="B105">
         <v>40.5</v>
       </c>
+      <c r="D105">
+        <v>102</v>
+      </c>
+      <c r="E105">
+        <v>68.25</v>
+      </c>
       <c r="J105">
         <v>52</v>
       </c>
@@ -31247,6 +33434,12 @@
       <c r="B106">
         <v>40.75</v>
       </c>
+      <c r="D106">
+        <v>102.5</v>
+      </c>
+      <c r="E106">
+        <v>68.5</v>
+      </c>
       <c r="J106">
         <v>52.5</v>
       </c>
@@ -31261,6 +33454,12 @@
       <c r="B107">
         <v>41</v>
       </c>
+      <c r="D107">
+        <v>103</v>
+      </c>
+      <c r="E107">
+        <v>68.75</v>
+      </c>
       <c r="J107">
         <v>53</v>
       </c>
@@ -31275,6 +33474,12 @@
       <c r="B108">
         <v>41.25</v>
       </c>
+      <c r="D108">
+        <v>103.5</v>
+      </c>
+      <c r="E108">
+        <v>69.25</v>
+      </c>
       <c r="J108">
         <v>53.5</v>
       </c>
@@ -31289,6 +33494,12 @@
       <c r="B109">
         <v>41.5</v>
       </c>
+      <c r="D109">
+        <v>104</v>
+      </c>
+      <c r="E109">
+        <v>69.5</v>
+      </c>
       <c r="J109">
         <v>54</v>
       </c>
@@ -31303,6 +33514,12 @@
       <c r="B110">
         <v>41.5</v>
       </c>
+      <c r="D110">
+        <v>104.5</v>
+      </c>
+      <c r="E110">
+        <v>70</v>
+      </c>
       <c r="J110">
         <v>54.5</v>
       </c>
@@ -31317,6 +33534,12 @@
       <c r="B111">
         <v>41.75</v>
       </c>
+      <c r="D111">
+        <v>105</v>
+      </c>
+      <c r="E111">
+        <v>70.25</v>
+      </c>
       <c r="J111">
         <v>55</v>
       </c>
@@ -31331,6 +33554,12 @@
       <c r="B112">
         <v>42</v>
       </c>
+      <c r="D112">
+        <v>105.5</v>
+      </c>
+      <c r="E112">
+        <v>70.5</v>
+      </c>
       <c r="J112">
         <v>55.5</v>
       </c>
@@ -31345,6 +33574,12 @@
       <c r="B113">
         <v>42.25</v>
       </c>
+      <c r="D113">
+        <v>106</v>
+      </c>
+      <c r="E113">
+        <v>70.75</v>
+      </c>
       <c r="J113">
         <v>56</v>
       </c>
@@ -31359,6 +33594,12 @@
       <c r="B114">
         <v>42.5</v>
       </c>
+      <c r="D114">
+        <v>106.5</v>
+      </c>
+      <c r="E114">
+        <v>71.25</v>
+      </c>
       <c r="J114">
         <v>56.5</v>
       </c>
@@ -31373,6 +33614,12 @@
       <c r="B115">
         <v>42.5</v>
       </c>
+      <c r="D115">
+        <v>107</v>
+      </c>
+      <c r="E115">
+        <v>71.5</v>
+      </c>
       <c r="J115">
         <v>57</v>
       </c>
@@ -31387,6 +33634,12 @@
       <c r="B116">
         <v>43</v>
       </c>
+      <c r="D116">
+        <v>107.5</v>
+      </c>
+      <c r="E116">
+        <v>71.75</v>
+      </c>
       <c r="J116">
         <v>57.5</v>
       </c>
@@ -31401,6 +33654,12 @@
       <c r="B117">
         <v>43</v>
       </c>
+      <c r="D117">
+        <v>108</v>
+      </c>
+      <c r="E117">
+        <v>72</v>
+      </c>
       <c r="J117">
         <v>58</v>
       </c>
@@ -31415,6 +33674,12 @@
       <c r="B118">
         <v>43.25</v>
       </c>
+      <c r="D118">
+        <v>108.5</v>
+      </c>
+      <c r="E118">
+        <v>72.25</v>
+      </c>
       <c r="J118">
         <v>58.5</v>
       </c>
@@ -31429,6 +33694,12 @@
       <c r="B119">
         <v>43.5</v>
       </c>
+      <c r="D119">
+        <v>109</v>
+      </c>
+      <c r="E119">
+        <v>72.5</v>
+      </c>
       <c r="J119">
         <v>59</v>
       </c>
@@ -31443,6 +33714,12 @@
       <c r="B120">
         <v>44</v>
       </c>
+      <c r="D120">
+        <v>109.5</v>
+      </c>
+      <c r="E120">
+        <v>73</v>
+      </c>
       <c r="J120">
         <v>59.5</v>
       </c>
@@ -31457,6 +33734,12 @@
       <c r="B121">
         <v>44</v>
       </c>
+      <c r="D121">
+        <v>110</v>
+      </c>
+      <c r="E121">
+        <v>73.25</v>
+      </c>
       <c r="J121">
         <v>60</v>
       </c>
@@ -31471,6 +33754,12 @@
       <c r="B122">
         <v>44.25</v>
       </c>
+      <c r="D122">
+        <v>110.51</v>
+      </c>
+      <c r="E122">
+        <v>73.5</v>
+      </c>
       <c r="J122">
         <v>60.5</v>
       </c>
@@ -31485,6 +33774,12 @@
       <c r="B123">
         <v>44.5</v>
       </c>
+      <c r="D123">
+        <v>111.01</v>
+      </c>
+      <c r="E123">
+        <v>73.75</v>
+      </c>
       <c r="J123">
         <v>61</v>
       </c>
@@ -31499,6 +33794,12 @@
       <c r="B124">
         <v>44.75</v>
       </c>
+      <c r="D124">
+        <v>111.51</v>
+      </c>
+      <c r="E124">
+        <v>74</v>
+      </c>
       <c r="J124">
         <v>61.5</v>
       </c>
@@ -31513,6 +33814,12 @@
       <c r="B125">
         <v>45</v>
       </c>
+      <c r="D125">
+        <v>112.01</v>
+      </c>
+      <c r="E125">
+        <v>74.25</v>
+      </c>
       <c r="J125">
         <v>62</v>
       </c>
@@ -31527,6 +33834,12 @@
       <c r="B126">
         <v>45.25</v>
       </c>
+      <c r="D126">
+        <v>112.51</v>
+      </c>
+      <c r="E126">
+        <v>74.75</v>
+      </c>
       <c r="J126">
         <v>62.5</v>
       </c>
@@ -31541,6 +33854,12 @@
       <c r="B127">
         <v>45.5</v>
       </c>
+      <c r="D127">
+        <v>113.01</v>
+      </c>
+      <c r="E127">
+        <v>75</v>
+      </c>
       <c r="J127">
         <v>63</v>
       </c>
@@ -31555,6 +33874,12 @@
       <c r="B128">
         <v>45.75</v>
       </c>
+      <c r="D128">
+        <v>113.51</v>
+      </c>
+      <c r="E128">
+        <v>75.25</v>
+      </c>
       <c r="J128">
         <v>63.5</v>
       </c>
@@ -31569,6 +33894,12 @@
       <c r="B129">
         <v>46</v>
       </c>
+      <c r="D129">
+        <v>114.01</v>
+      </c>
+      <c r="E129">
+        <v>75.5</v>
+      </c>
       <c r="J129">
         <v>64</v>
       </c>
@@ -31583,6 +33914,12 @@
       <c r="B130">
         <v>46.25</v>
       </c>
+      <c r="D130">
+        <v>114.51</v>
+      </c>
+      <c r="E130">
+        <v>75.75</v>
+      </c>
       <c r="J130">
         <v>64.5</v>
       </c>
@@ -31597,6 +33934,12 @@
       <c r="B131">
         <v>46.5</v>
       </c>
+      <c r="D131">
+        <v>115.01</v>
+      </c>
+      <c r="E131">
+        <v>76.25</v>
+      </c>
       <c r="J131">
         <v>65</v>
       </c>
@@ -31611,6 +33954,12 @@
       <c r="B132">
         <v>46.75</v>
       </c>
+      <c r="D132">
+        <v>115.51</v>
+      </c>
+      <c r="E132">
+        <v>76.5</v>
+      </c>
       <c r="J132">
         <v>65.5</v>
       </c>
@@ -31625,6 +33974,12 @@
       <c r="B133">
         <v>47</v>
       </c>
+      <c r="D133">
+        <v>116.01</v>
+      </c>
+      <c r="E133">
+        <v>76.75</v>
+      </c>
       <c r="J133">
         <v>66</v>
       </c>
@@ -31639,6 +33994,12 @@
       <c r="B134">
         <v>47.25</v>
       </c>
+      <c r="D134">
+        <v>116.51</v>
+      </c>
+      <c r="E134">
+        <v>77.25</v>
+      </c>
       <c r="J134">
         <v>66.5</v>
       </c>
@@ -31653,6 +34014,12 @@
       <c r="B135">
         <v>47.5</v>
       </c>
+      <c r="D135">
+        <v>117.01</v>
+      </c>
+      <c r="E135">
+        <v>77.5</v>
+      </c>
       <c r="J135">
         <v>67</v>
       </c>
@@ -31667,6 +34034,12 @@
       <c r="B136">
         <v>47.75</v>
       </c>
+      <c r="D136">
+        <v>117.51</v>
+      </c>
+      <c r="E136">
+        <v>77.75</v>
+      </c>
       <c r="J136">
         <v>67.5</v>
       </c>
@@ -31681,6 +34054,12 @@
       <c r="B137">
         <v>48.25</v>
       </c>
+      <c r="D137">
+        <v>118.01</v>
+      </c>
+      <c r="E137">
+        <v>78</v>
+      </c>
       <c r="J137">
         <v>68</v>
       </c>
@@ -31695,6 +34074,12 @@
       <c r="B138">
         <v>48.25</v>
       </c>
+      <c r="D138">
+        <v>118.51</v>
+      </c>
+      <c r="E138">
+        <v>78.5</v>
+      </c>
       <c r="J138">
         <v>68.5</v>
       </c>
@@ -31709,6 +34094,12 @@
       <c r="B139">
         <v>48.75</v>
       </c>
+      <c r="D139">
+        <v>119.01</v>
+      </c>
+      <c r="E139">
+        <v>78.75</v>
+      </c>
       <c r="J139">
         <v>69</v>
       </c>
@@ -31723,6 +34114,12 @@
       <c r="B140">
         <v>48.75</v>
       </c>
+      <c r="D140">
+        <v>119.51</v>
+      </c>
+      <c r="E140">
+        <v>79</v>
+      </c>
       <c r="J140">
         <v>69.5</v>
       </c>
@@ -31737,6 +34134,12 @@
       <c r="B141">
         <v>49.25</v>
       </c>
+      <c r="D141">
+        <v>120.01</v>
+      </c>
+      <c r="E141">
+        <v>79.25</v>
+      </c>
       <c r="J141">
         <v>70</v>
       </c>
@@ -31751,6 +34154,12 @@
       <c r="B142">
         <v>49.25</v>
       </c>
+      <c r="D142">
+        <v>120.51</v>
+      </c>
+      <c r="E142">
+        <v>79.5</v>
+      </c>
       <c r="J142">
         <v>70.5</v>
       </c>
@@ -31764,6 +34173,12 @@
       </c>
       <c r="B143">
         <v>49.75</v>
+      </c>
+      <c r="D143">
+        <v>121.01</v>
+      </c>
+      <c r="E143">
+        <v>79.75</v>
       </c>
       <c r="J143">
         <v>71</v>

</xml_diff>